<commit_message>
Changes ConfigListener, ImportExcel Customer
</commit_message>
<xml_diff>
--- a/config-properties/Sample_upload_cust.xlsx
+++ b/config-properties/Sample_upload_cust.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29127"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\micro-service-Workspace\banking-app\config-properties\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{29EADE69-CD4F-41DE-B92B-4022FE60188C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AA294831-42C0-4513-9979-2CC0A9D74C26}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{B51642AB-44C8-4557-8199-2E3C1B6BE0ED}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="66">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="78">
   <si>
     <t>CUSTOMER_TITLE</t>
   </si>
@@ -234,6 +234,42 @@
   </si>
   <si>
     <t>INR</t>
+  </si>
+  <si>
+    <t>BUDDHA KATHERA</t>
+  </si>
+  <si>
+    <t>KANCHAN SINGH</t>
+  </si>
+  <si>
+    <t>PASSPORT_ISSUE_DATE</t>
+  </si>
+  <si>
+    <t>Sahanawali</t>
+  </si>
+  <si>
+    <t>Burawai</t>
+  </si>
+  <si>
+    <t>Rajasthan</t>
+  </si>
+  <si>
+    <t>Bharatpur</t>
+  </si>
+  <si>
+    <t>LOCAL</t>
+  </si>
+  <si>
+    <t>BUSINESS</t>
+  </si>
+  <si>
+    <t>33-35</t>
+  </si>
+  <si>
+    <t>VKIA-Road No 9</t>
+  </si>
+  <si>
+    <t>Jaipur</t>
   </si>
 </sst>
 </file>
@@ -304,9 +340,6 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="14" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="49" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
@@ -314,10 +347,13 @@
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -655,50 +691,55 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{07F75C49-BF20-49B5-9D49-5DFAE25244FF}">
-  <dimension ref="A1:AY3"/>
+  <dimension ref="A1:AZ3"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="I12" sqref="I12"/>
+    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="AQ1" sqref="AQ1:AQ1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
   <cols>
-    <col min="1" max="1" width="14.08984375" style="7" customWidth="1"/>
+    <col min="1" max="1" width="14.08984375" style="6" customWidth="1"/>
     <col min="2" max="2" width="15.7265625" customWidth="1"/>
     <col min="3" max="5" width="13" customWidth="1"/>
     <col min="6" max="6" width="12.36328125" customWidth="1"/>
     <col min="7" max="7" width="14.08984375" customWidth="1"/>
     <col min="8" max="8" width="12.36328125" customWidth="1"/>
-    <col min="9" max="9" width="14.08984375" style="12" customWidth="1"/>
+    <col min="9" max="9" width="14.08984375" style="11" customWidth="1"/>
     <col min="10" max="11" width="12.36328125" customWidth="1"/>
-    <col min="12" max="12" width="13" style="4" customWidth="1"/>
-    <col min="13" max="13" width="16.08984375" style="7" customWidth="1"/>
+    <col min="12" max="12" width="13" style="6" customWidth="1"/>
+    <col min="13" max="13" width="16.08984375" style="6" customWidth="1"/>
     <col min="14" max="14" width="13" customWidth="1"/>
-    <col min="15" max="17" width="14.08984375" customWidth="1"/>
-    <col min="18" max="20" width="13" customWidth="1"/>
-    <col min="21" max="25" width="14.08984375" style="12" customWidth="1"/>
-    <col min="26" max="26" width="16.81640625" style="12" customWidth="1"/>
-    <col min="27" max="27" width="12.7265625" style="12" customWidth="1"/>
-    <col min="28" max="30" width="11.26953125" style="12" customWidth="1"/>
-    <col min="31" max="32" width="14.08984375" style="12" customWidth="1"/>
-    <col min="33" max="33" width="14.81640625" style="12" customWidth="1"/>
-    <col min="34" max="34" width="23.6328125" style="12" customWidth="1"/>
-    <col min="35" max="35" width="14.36328125" customWidth="1"/>
-    <col min="36" max="36" width="15" customWidth="1"/>
-    <col min="37" max="37" width="14.08984375" customWidth="1"/>
-    <col min="38" max="38" width="17" customWidth="1"/>
-    <col min="39" max="39" width="11.54296875" customWidth="1"/>
-    <col min="40" max="40" width="13.1796875" customWidth="1"/>
+    <col min="15" max="18" width="14.08984375" customWidth="1"/>
+    <col min="19" max="21" width="13" customWidth="1"/>
+    <col min="22" max="26" width="14.08984375" style="11" customWidth="1"/>
+    <col min="27" max="27" width="16.81640625" style="11" customWidth="1"/>
+    <col min="28" max="28" width="12.7265625" style="11" customWidth="1"/>
+    <col min="29" max="31" width="11.26953125" style="11" customWidth="1"/>
+    <col min="32" max="33" width="14.08984375" style="11" customWidth="1"/>
+    <col min="34" max="34" width="20.08984375" style="11" customWidth="1"/>
+    <col min="35" max="35" width="23.6328125" style="11" customWidth="1"/>
+    <col min="36" max="36" width="15.7265625" customWidth="1"/>
+    <col min="37" max="37" width="16.26953125" customWidth="1"/>
+    <col min="38" max="38" width="14.08984375" customWidth="1"/>
+    <col min="39" max="39" width="17" customWidth="1"/>
+    <col min="40" max="40" width="11.54296875" customWidth="1"/>
     <col min="41" max="41" width="12.81640625" customWidth="1"/>
-    <col min="42" max="43" width="12.54296875" customWidth="1"/>
-    <col min="44" max="44" width="12.81640625" customWidth="1"/>
-    <col min="45" max="45" width="12.7265625" customWidth="1"/>
-    <col min="46" max="46" width="14.81640625" customWidth="1"/>
-    <col min="47" max="47" width="13.90625" customWidth="1"/>
+    <col min="42" max="42" width="13.1796875" customWidth="1"/>
+    <col min="43" max="43" width="12.54296875" customWidth="1"/>
+    <col min="44" max="44" width="25" customWidth="1"/>
+    <col min="45" max="45" width="20.6328125" customWidth="1"/>
+    <col min="46" max="46" width="18.36328125" customWidth="1"/>
+    <col min="47" max="47" width="18.54296875" customWidth="1"/>
+    <col min="48" max="48" width="15.453125" customWidth="1"/>
+    <col min="49" max="49" width="12.54296875" customWidth="1"/>
+    <col min="50" max="50" width="10.90625" customWidth="1"/>
+    <col min="51" max="51" width="14.1796875" customWidth="1"/>
+    <col min="52" max="52" width="10.54296875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:51" s="2" customFormat="1">
-      <c r="A1" s="6" t="s">
+    <row r="1" spans="1:52" s="2" customFormat="1">
+      <c r="A1" s="5" t="s">
         <v>46</v>
       </c>
       <c r="B1" s="2" t="s">
@@ -725,16 +766,16 @@
       <c r="I1" s="1" t="s">
         <v>57</v>
       </c>
-      <c r="J1" s="11" t="s">
+      <c r="J1" s="10" t="s">
         <v>40</v>
       </c>
       <c r="K1" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="L1" s="3" t="s">
+      <c r="L1" s="12" t="s">
         <v>7</v>
       </c>
-      <c r="M1" s="6" t="s">
+      <c r="M1" s="5" t="s">
         <v>9</v>
       </c>
       <c r="N1" s="2" t="s">
@@ -747,119 +788,122 @@
         <v>55</v>
       </c>
       <c r="Q1" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="R1" s="2" t="s">
         <v>56</v>
       </c>
-      <c r="R1" s="2" t="s">
+      <c r="S1" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="S1" s="2" t="s">
+      <c r="T1" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="T1" s="2" t="s">
+      <c r="U1" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="U1" s="1" t="s">
+      <c r="V1" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="V1" s="1" t="s">
+      <c r="W1" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="W1" s="1" t="s">
+      <c r="X1" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="X1" s="1" t="s">
+      <c r="Y1" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="Y1" s="1" t="s">
+      <c r="Z1" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="Z1" s="1" t="s">
+      <c r="AA1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="AA1" s="1" t="s">
+      <c r="AB1" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="AB1" s="1" t="s">
+      <c r="AC1" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="AC1" s="1" t="s">
+      <c r="AD1" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="AD1" s="1" t="s">
+      <c r="AE1" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="AE1" s="1" t="s">
+      <c r="AF1" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="AF1" s="1" t="s">
+      <c r="AG1" s="1" t="s">
         <v>64</v>
       </c>
-      <c r="AG1" s="1" t="s">
+      <c r="AH1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="AH1" s="1" t="s">
+      <c r="AI1" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="AI1" s="2" t="s">
+      <c r="AJ1" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="AJ1" s="2" t="s">
+      <c r="AK1" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="AK1" s="2" t="s">
+      <c r="AL1" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="AL1" s="2" t="s">
+      <c r="AM1" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="AM1" s="2" t="s">
+      <c r="AN1" s="2" t="s">
         <v>18</v>
-      </c>
-      <c r="AN1" s="2" t="s">
-        <v>19</v>
       </c>
       <c r="AO1" s="2" t="s">
         <v>20</v>
       </c>
       <c r="AP1" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="AQ1" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="AQ1" s="2" t="s">
+      <c r="AR1" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="AR1" s="2" t="s">
+      <c r="AS1" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="AS1" s="2" t="s">
+      <c r="AT1" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="AT1" s="2" t="s">
+      <c r="AU1" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="AU1" s="2" t="s">
+      <c r="AV1" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="AV1" s="2" t="s">
+      <c r="AW1" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="AW1" s="2" t="s">
+      <c r="AX1" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="AX1" s="2" t="s">
+      <c r="AY1" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="AY1" s="2" t="s">
+      <c r="AZ1" s="2" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="2" spans="1:51">
-      <c r="A2" s="7" t="s">
+    <row r="2" spans="1:52">
+      <c r="A2" s="6" t="s">
         <v>63</v>
       </c>
       <c r="B2" t="s">
         <v>22</v>
       </c>
-      <c r="C2" s="5" t="s">
+      <c r="C2" s="4" t="s">
         <v>23</v>
       </c>
       <c r="E2" t="s">
@@ -874,51 +918,87 @@
       <c r="H2" t="s">
         <v>39</v>
       </c>
-      <c r="I2" s="12" t="s">
+      <c r="I2" s="11" t="s">
         <v>22</v>
       </c>
-      <c r="L2" s="4">
+      <c r="J2" t="s">
+        <v>66</v>
+      </c>
+      <c r="L2" s="3">
         <v>26258</v>
       </c>
-      <c r="M2" s="8" t="s">
+      <c r="M2" s="7" t="s">
         <v>27</v>
       </c>
       <c r="N2" t="s">
         <v>29</v>
       </c>
-      <c r="R2">
-        <v>1234567890</v>
-      </c>
-      <c r="T2" s="10" t="s">
+      <c r="S2">
+        <v>9660356475</v>
+      </c>
+      <c r="U2" s="9" t="s">
         <v>31</v>
       </c>
-      <c r="U2" s="12" t="s">
+      <c r="V2" s="11" t="s">
         <v>61</v>
       </c>
-      <c r="AA2" s="12" t="s">
+      <c r="AB2" s="11" t="s">
         <v>33</v>
       </c>
-      <c r="AB2" s="12" t="s">
+      <c r="AC2" s="11" t="s">
         <v>44</v>
       </c>
-      <c r="AC2" s="12" t="s">
+      <c r="AD2" s="11" t="s">
         <v>45</v>
       </c>
-      <c r="AF2" s="12" t="s">
+      <c r="AG2" s="11" t="s">
         <v>65</v>
       </c>
-      <c r="AH2" s="12" t="s">
+      <c r="AI2" s="11" t="s">
         <v>34</v>
       </c>
+      <c r="AJ2">
+        <v>102</v>
+      </c>
+      <c r="AK2" t="s">
+        <v>69</v>
+      </c>
+      <c r="AO2" t="s">
+        <v>71</v>
+      </c>
+      <c r="AP2" t="s">
+        <v>72</v>
+      </c>
+      <c r="AQ2">
+        <v>302022</v>
+      </c>
+      <c r="AR2" t="s">
+        <v>73</v>
+      </c>
+      <c r="AS2">
+        <v>102</v>
+      </c>
+      <c r="AT2" t="s">
+        <v>69</v>
+      </c>
+      <c r="AX2" t="s">
+        <v>71</v>
+      </c>
+      <c r="AY2" t="s">
+        <v>72</v>
+      </c>
+      <c r="AZ2">
+        <v>302022</v>
+      </c>
     </row>
-    <row r="3" spans="1:51">
-      <c r="A3" s="7" t="s">
+    <row r="3" spans="1:52">
+      <c r="A3" s="6" t="s">
         <v>63</v>
       </c>
       <c r="B3" t="s">
         <v>22</v>
       </c>
-      <c r="C3" s="5" t="s">
+      <c r="C3" s="4" t="s">
         <v>25</v>
       </c>
       <c r="E3" t="s">
@@ -933,38 +1013,74 @@
       <c r="H3" t="s">
         <v>60</v>
       </c>
-      <c r="I3" s="12" t="s">
+      <c r="I3" s="11" t="s">
         <v>22</v>
       </c>
-      <c r="L3" s="4">
+      <c r="J3" t="s">
+        <v>67</v>
+      </c>
+      <c r="L3" s="3">
         <v>26259</v>
       </c>
-      <c r="M3" s="9" t="s">
+      <c r="M3" s="8" t="s">
         <v>28</v>
       </c>
       <c r="N3" t="s">
         <v>30</v>
       </c>
-      <c r="R3">
-        <v>1234567890</v>
-      </c>
-      <c r="U3" s="12" t="s">
+      <c r="S3">
+        <v>9571758945</v>
+      </c>
+      <c r="V3" s="11" t="s">
         <v>62</v>
       </c>
-      <c r="AA3" s="12" t="s">
+      <c r="AB3" s="11" t="s">
         <v>33</v>
       </c>
-      <c r="AB3" s="12" t="s">
+      <c r="AC3" s="11" t="s">
         <v>44</v>
       </c>
-      <c r="AC3" s="12" t="s">
+      <c r="AD3" s="11" t="s">
         <v>45</v>
       </c>
-      <c r="AF3" s="12" t="s">
+      <c r="AG3" s="11" t="s">
         <v>65</v>
       </c>
-      <c r="AH3" s="12" t="s">
+      <c r="AI3" s="11" t="s">
         <v>34</v>
+      </c>
+      <c r="AJ3">
+        <v>103</v>
+      </c>
+      <c r="AK3" t="s">
+        <v>70</v>
+      </c>
+      <c r="AO3" t="s">
+        <v>71</v>
+      </c>
+      <c r="AP3" t="s">
+        <v>72</v>
+      </c>
+      <c r="AQ3">
+        <v>302017</v>
+      </c>
+      <c r="AR3" t="s">
+        <v>74</v>
+      </c>
+      <c r="AS3" t="s">
+        <v>75</v>
+      </c>
+      <c r="AT3" t="s">
+        <v>76</v>
+      </c>
+      <c r="AX3" t="s">
+        <v>71</v>
+      </c>
+      <c r="AY3" t="s">
+        <v>77</v>
+      </c>
+      <c r="AZ3">
+        <v>302017</v>
       </c>
     </row>
   </sheetData>
@@ -972,13 +1088,13 @@
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Select Customer Title" sqref="B1:B1048576" xr:uid="{8FF3B3B0-FF0A-4538-8ACB-0C0B4A3AF1DC}">
       <formula1>"Mr.,Mrs.,Ms.,Mx.,Dr."</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Select  Customer Constitution" sqref="AA1:AA1048576" xr:uid="{6769CDB8-B687-4D3D-A264-3078FF520F52}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Select  Customer Constitution" sqref="AB1:AB1048576" xr:uid="{6769CDB8-B687-4D3D-A264-3078FF520F52}">
       <formula1>"GEN, INDV, JNT, ILL, BLD, DAD, HND, PRD, HUF, CNS, PRS, NPS, SOP, JSE, RPT, URP, POC, PSU, GOU, RSO, URS, COS, PTR, PUT, CLB, PVT, PLC, GOV, SGA, GDE, BNK, FCM, NCL, ASS, INS, NIT, NAP"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AH1:AH1048576" xr:uid="{E6CB8705-E85C-487D-A706-A020AB7BB21A}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AI1:AI1048576" xr:uid="{E6CB8705-E85C-487D-A706-A020AB7BB21A}">
       <formula1>"PERMANENT"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AQ1:AQ1048576" xr:uid="{78F1655F-EEB4-4753-8693-07BFC306AB48}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AR1:AR1048576" xr:uid="{78F1655F-EEB4-4753-8693-07BFC306AB48}">
       <formula1>"LOCAL,BUSINESS"</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F1:F1048576" xr:uid="{049E07A7-F7A0-41FF-9ECF-C6D6A0D8AFCB}">
@@ -987,33 +1103,33 @@
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H1:H1048576" xr:uid="{151DC8D6-9DA9-4462-9510-AE17DFC9BDE6}">
       <formula1>"Father ,Wife ,Son ,Daughter"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AB1:AB1048576" xr:uid="{58C9E668-6171-4F52-AD16-D50F54B318AE}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AC1:AC1048576" xr:uid="{58C9E668-6171-4F52-AD16-D50F54B318AE}">
       <formula1>"HIN, MUS, JAI, CHR, SIK"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AC1:AC1048576" xr:uid="{9E57A22A-6492-4BFC-A0F2-79261A54C691}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AD1:AD1048576" xr:uid="{9E57A22A-6492-4BFC-A0F2-79261A54C691}">
       <formula1>"GEN ,SC ,ST ,OBC"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AX1:AX1048576" xr:uid="{6A530A7B-9D9F-47D1-9DE1-DEAC783E1EEE}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AY1 AY4:AY1048576" xr:uid="{6A530A7B-9D9F-47D1-9DE1-DEAC783E1EEE}">
       <formula1>"AP, AR, AS, BR, CG, GA, GJ, HR, HP, JH, KA, KL, MP, MH, MN, ML, MZ, NL, OD, PB, RJ, SK, TN, TS, TR, UP, UK, WB, AN, CH, DD, DL, JK, LD, LK, PY"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G1:G1048576 G1:G1048576" xr:uid="{E89458DC-12AB-4634-8C87-E4047FB95613}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G1:G1048576" xr:uid="{E89458DC-12AB-4634-8C87-E4047FB95613}">
       <formula1>"MARRIED,UNMARRIED"</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="I1:I1048576" xr:uid="{B98E2ABA-94C1-4CDE-9DC6-7DD4DB1AC387}">
       <formula1>"Mr.,Dr."</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="U1:U1048576" xr:uid="{AB38874D-37DE-48B9-A22B-954E6E9C2200}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="V1:V1048576" xr:uid="{AB38874D-37DE-48B9-A22B-954E6E9C2200}">
       <formula1>"Y,N"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="V1:V1048576 W1:W1048576" xr:uid="{A8905D35-BFBB-45E1-B84F-D676B2743EA9}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="W1:X1048576" xr:uid="{A8905D35-BFBB-45E1-B84F-D676B2743EA9}">
       <formula1>"N,Y"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AF1:AF1048576" xr:uid="{17630511-B36E-4D9B-A1C4-A08E70CAB146}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AG1:AG1048576" xr:uid="{17630511-B36E-4D9B-A1C4-A08E70CAB146}">
       <formula1>"INR"</formula1>
     </dataValidation>
   </dataValidations>
   <hyperlinks>
-    <hyperlink ref="T2" r:id="rId1" xr:uid="{822F488B-ABC1-47C8-824D-E88D78CC8716}"/>
+    <hyperlink ref="U2" r:id="rId1" xr:uid="{822F488B-ABC1-47C8-824D-E88D78CC8716}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>